<commit_message>
updated print to excel functions and ship parallels
</commit_message>
<xml_diff>
--- a/shipClassTests/test_ship_data.xlsx
+++ b/shipClassTests/test_ship_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adware\Desktop\KISS\shipClassTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828EA159-0667-4FE6-91FF-6A3538250E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2142F9-62CB-4626-91F3-71120CCAECB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comp_rel_data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="system_structures" sheetId="2" r:id="rId2"/>
+    <sheet name="ship_structure" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>python idx</t>
   </si>
@@ -86,6 +87,18 @@
   </si>
   <si>
     <t>[([4,5], [6,7]), (0,1)]</t>
+  </si>
+  <si>
+    <t>ship structure</t>
+  </si>
+  <si>
+    <t>[(1,2), (3,4)]</t>
+  </si>
+  <si>
+    <t>complex sys 2</t>
+  </si>
+  <si>
+    <t>[([0,4], [1,5]), (6,7)]</t>
   </si>
 </sst>
 </file>
@@ -421,13 +434,13 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.53125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -455,7 +468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -469,7 +482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -483,7 +496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -497,7 +510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -511,7 +524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -525,7 +538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -539,7 +552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -560,18 +573,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980DD151-C602-4BC7-B6E1-6E9BEFCC586A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.265625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -579,7 +592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -587,7 +600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -595,12 +608,45 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3717880F-B210-47BE-954D-9ABA10FB260E}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>